<commit_message>
Updated Lab-02 (MP, all tasks)
</commit_message>
<xml_diff>
--- a/MP/Lab-02/Graphs.xlsx
+++ b/MP/Lab-02/Graphs.xlsx
@@ -5,18 +5,21 @@
   <fileSharing readOnlyRecommended="0" userName="unknow"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="3" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Salesman" sheetId="1" r:id="rId3"/>
+    <sheet name="Knapsack" sheetId="2" r:id="rId4"/>
+    <sheet name="Boat" sheetId="3" r:id="rId5"/>
+    <sheet name="Boat_c" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1656713618" val="1046" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1656713618" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1656713618"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1656713618"/>
+      <pm:revision xmlns:pm="smNativeData" day="1656783402" val="1046" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1656783402" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1656783402" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1656783402"/>
     </ext>
   </extLst>
 </workbook>
@@ -24,7 +27,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="17">
+  <numFmts count="22">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
@@ -42,6 +45,11 @@
     <numFmt numFmtId="168" formatCode="0.000000"/>
     <numFmt numFmtId="169" formatCode="0.0000000"/>
     <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="171" formatCode="0.000000000"/>
+    <numFmt numFmtId="172" formatCode="0.0000000000"/>
+    <numFmt numFmtId="173" formatCode="0.00000000000"/>
+    <numFmt numFmtId="174" formatCode="0.000000000000"/>
+    <numFmt numFmtId="175" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -51,7 +59,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1656713618" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1656783402" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -66,7 +74,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1656713618" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1656783402" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -88,7 +96,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1656713618" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1656783402" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -110,7 +118,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1656713618"/>
+          <pm:border xmlns:pm="smNativeData" id="1656783402"/>
         </ext>
       </extLst>
     </border>
@@ -129,7 +137,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1656713618"/>
+          <pm:border xmlns:pm="smNativeData" id="1656783402"/>
         </ext>
       </extLst>
     </border>
@@ -137,9 +145,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -147,7 +156,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1656713618" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1656783402" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -161,7 +170,35 @@
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="1995" b="1" i="0" u="none" strike="noStrike" kern="100">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>Зависимость времени выполнения от количества городов</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -184,16 +221,22 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-us" sz="1500" b="0" i="0" u="none" strike="noStrike">
+                  <a:defRPr lang="en-us" sz="1500" b="0" i="0" u="none" strike="noStrike" kern="100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="Basic Sans"/>
+                    <a:latin typeface="Basic Sans" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
@@ -268,6 +311,286 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>61.846262735</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:sm="smo" uri="smo">
+              <sm:meanLine>
+                <c:spPr>
+                  <a:ln w="9525">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:meanLine>
+              <sm:minMaxLine>
+                <c:spPr>
+                  <a:ln w="9525">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:minMaxLine>
+              <sm:stDevLine>
+                <c:spPr>
+                  <a:ln w="9525">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:stDevLine>
+              <sm:trendLine>
+                <c:spPr>
+                  <a:ln w="9525">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:trendLine>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:extLst>
+          <c:ext xmlns:sm="smo" uri="smo">
+            <sm:boxPlot xmlns:sm="smo" val="0"/>
+            <sm:turned xmlns:sm="smo" val="0"/>
+          </c:ext>
+        </c:extLst>
+        <c:axId val="10"/>
+        <c:axId val="11"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="11"/>
+        <c:crosses val="max"/>
+        <c:auto val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="11"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-us" sz="1995" b="1" i="0" u="none" strike="noStrike" kern="100">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Basic Sans" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>Время, с</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr/>
+  <c:txPr>
+    <a:bodyPr anchor="ctr" anchorCtr="1" rot="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-us" sz="1995" b="0" i="0" u="none" strike="noStrike" kern="100">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Basic Sans" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext xmlns:sm="smo" uri="smo">
+      <sm:colorScheme xmlns:sm="smo" id="1656783402" val="7"/>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="2295" b="1" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>Зависимость времени выполнения от количество мест в рюкзаке</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>t(items)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Knapsack!$A$1:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Knapsack!$B$1:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.001266171</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.002443925</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.007287561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.011906131</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.041093413</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.066096387</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.129045875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.269722808</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.548242751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -335,14 +658,14 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-us" sz="1995" b="0" i="0" u="none" strike="noStrike">
+              <a:defRPr lang="en-us" sz="2295" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -352,7 +675,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="11"/>
-        <c:crosses val="max"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
       </c:catAx>
       <c:valAx>
@@ -364,6 +687,34 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-us" sz="2295" b="1" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Basic Sans" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>Время, с</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
@@ -373,7 +724,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-us" sz="1995" b="0" i="0" u="none" strike="noStrike">
+              <a:defRPr lang="en-us" sz="2295" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -396,7 +747,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr lang="en-us" sz="1995" b="0" i="0" u="none" strike="noStrike">
+            <a:defRPr lang="en-us" sz="2295" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -415,7 +766,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr lang="en-us" sz="1995" b="0" i="0" u="none" strike="noStrike">
+        <a:defRPr lang="en-us" sz="2295" b="0" i="0" u="none" strike="noStrike">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -426,7 +777,642 @@
   </c:txPr>
   <c:extLst>
     <c:ext xmlns:sm="smo" uri="smo">
-      <sm:colorScheme xmlns:sm="smo" id="1656713618" val="7"/>
+      <sm:colorScheme xmlns:sm="smo" id="1656783402" val="7"/>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="2305" b="1" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>Зависимость времени выполнения от количества контейнеров</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>t(containers)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3F6898"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-us" sz="1000" b="0" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Basic Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Boat!$A$1:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Boat!$B$1:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.223577228</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34497532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.689237714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.314980034</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.219262191</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.269242395</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.453471214</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.417006949</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.457363441</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66.808302268</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>139.443602664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:sm="smo" uri="smo">
+              <sm:meanLine>
+                <c:spPr>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:meanLine>
+              <sm:minMaxLine>
+                <c:spPr>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:minMaxLine>
+              <sm:stDevLine>
+                <c:spPr>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:stDevLine>
+              <sm:trendLine>
+                <c:spPr>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:trendLine>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:extLst>
+          <c:ext xmlns:sm="smo" uri="smo">
+            <sm:boxPlot xmlns:sm="smo" val="0"/>
+            <sm:turned xmlns:sm="smo" val="0"/>
+          </c:ext>
+        </c:extLst>
+        <c:axId val="10"/>
+        <c:axId val="11"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="2305" b="0" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11"/>
+        <c:crosses val="max"/>
+        <c:auto val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="11"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-us" sz="2305" b="1" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Basic Sans" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>Время, с</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="2305" b="0" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-us" sz="2305" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Basic Sans" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr/>
+  <c:txPr>
+    <a:bodyPr anchor="ctr" anchorCtr="1" rot="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-us" sz="2305" b="0" i="0" u="none" strike="noStrike">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Basic Sans"/>
+        </a:defRPr>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext xmlns:sm="smo" uri="smo">
+      <sm:colorScheme xmlns:sm="smo" id="1656783402" val="7"/>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="1945" b="1" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>Зависимость времени выполнения от количества мест на корабле</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>t(places)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Boat_c!$A$1:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Boat_c!$B$1:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.00293641</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.016871245</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.076169916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.269467953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.737257609</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:sm="smo" uri="smo">
+              <sm:meanLine>
+                <c:spPr>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:meanLine>
+              <sm:minMaxLine>
+                <c:spPr>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:minMaxLine>
+              <sm:stDevLine>
+                <c:spPr>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:stDevLine>
+              <sm:trendLine>
+                <c:spPr>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+              </sm:trendLine>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:extLst>
+          <c:ext xmlns:sm="smo" uri="smo">
+            <sm:boxPlot xmlns:sm="smo" val="0"/>
+            <sm:turned xmlns:sm="smo" val="0"/>
+          </c:ext>
+        </c:extLst>
+        <c:axId val="10"/>
+        <c:axId val="11"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="1945" b="0" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="11"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-us" sz="1945" b="1" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Basic Sans" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>Время, с</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-us" sz="1945" b="0" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Basic Sans" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-us" sz="1945" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Basic Sans" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr/>
+  <c:txPr>
+    <a:bodyPr anchor="ctr" anchorCtr="1" rot="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-us" sz="1945" b="0" i="0" u="none" strike="noStrike">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Basic Sans"/>
+        </a:defRPr>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:extLst>
+    <c:ext xmlns:sm="smo" uri="smo">
+      <sm:colorScheme xmlns:sm="smo" id="1656783402" val="7"/>
     </c:ext>
   </c:extLst>
 </c:chartSpace>
@@ -446,6 +1432,111 @@
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>39370</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>86995</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1270</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>58420</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>106045</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>154305</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -725,7 +1816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
@@ -779,7 +1870,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.579360954999999933</v>
+        <v>0.579360954999999844</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -808,7 +1899,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1656713618" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1656783402" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -817,15 +1908,347 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1656713618" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1656713618" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1656783402" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1656783402" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <drawing r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1656713618" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1656783402" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <cols>
+    <col min="2" max="2" width="19.324324" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>0.00126617099999999994</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0.00244392499999999968</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0.00728756099999999929</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>0.0119061309999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>0.0410934130000000053</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0.0660963869999999964</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="n">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.129045874999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="n">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0.269722807999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="n">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>0.548242750999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10"/>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1656783402" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1656783402" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1656783402" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1656783402" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <cols>
+    <col min="2" max="2" width="14.864865" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>0.223577227999999995</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0.344975319999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="n">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0.689237713999999979</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="n">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>1.31498003399999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="n">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>2.21926219099999988</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>4.26924239500000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="n">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>8.45347121400000034</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="n">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>17.417006949000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="n">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>33.4573634409999983</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="n">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>66.8083022680000056</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="n">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>139.443602663999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1656783402" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1656783402" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1656783402" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1656783402" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <cols>
+    <col min="2" max="2" width="14.864865" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>0.00293641000000000005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0.0168712450000000018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0.0761699160000000042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>0.269467952999999971</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="n">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>0.73725760900000008</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1656783402" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1656783402" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1656783402" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1656783402" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>